<commit_message>
System stable for USB communication. High current charging activated
</commit_message>
<xml_diff>
--- a/SkeletylLayout.xlsx
+++ b/SkeletylLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sin Asignar\Documents\NL\Prototypes\SkeletylLP\PublicRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039E042B-F8C9-4D69-ABEA-0852EC5DEBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F7F1A4-4457-4DC2-A6D9-8C4E369770D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{21ABE6FE-2F18-42B9-969D-DE820B442B37}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -442,17 +442,12 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -460,9 +455,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,10 +482,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -810,7 +804,7 @@
   <dimension ref="A2:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,24 +815,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
       <c r="L2" s="6"/>
-      <c r="O2" s="22"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="O2" s="19"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -859,7 +849,6 @@
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="14"/>
       <c r="H4" s="1" t="s">
         <v>18</v>
       </c>
@@ -881,29 +870,28 @@
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="14" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="14"/>
       <c r="H5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="14" t="s">
         <v>26</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -927,7 +915,6 @@
       <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="14"/>
       <c r="H6" s="1" t="s">
         <v>29</v>
       </c>
@@ -943,11 +930,10 @@
       <c r="L6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="14"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="D7" s="13" t="s">
+      <c r="A7" s="20"/>
+      <c r="D7" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -960,17 +946,17 @@
         <v>50</v>
       </c>
       <c r="I7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="20"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="20"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
@@ -978,10 +964,6 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G13" s="14"/>
-      <c r="O13" s="14"/>
-    </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>35</v>
@@ -1001,7 +983,6 @@
       <c r="F14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="14"/>
       <c r="H14" s="2">
         <v>6</v>
       </c>
@@ -1017,42 +998,40 @@
       <c r="L14" s="2">
         <v>0</v>
       </c>
-      <c r="O14" s="14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="15" t="s">
         <v>43</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="20" t="s">
+      <c r="G15" s="13"/>
+      <c r="H15" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="21" t="s">
+      <c r="I15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="J15" s="21" t="s">
+      <c r="J15" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="K15" s="21" t="s">
+      <c r="K15" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="L15" s="20" t="s">
+      <c r="L15" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="O15" s="14"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
@@ -1063,7 +1042,6 @@
       <c r="F16" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="14"/>
       <c r="H16" s="2">
         <v>1</v>
       </c>
@@ -1079,10 +1057,9 @@
       <c r="L16" s="2">
         <v>5</v>
       </c>
-      <c r="O16" s="14"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
       <c r="D17" s="8" t="s">
         <v>77</v>
       </c>
@@ -1096,44 +1073,29 @@
         <v>51</v>
       </c>
       <c r="I17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="O17" s="14"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="O18" s="14"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="O19" s="14"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O20" s="14"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O21" s="14"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O22" s="14"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O23" s="14"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="3" t="s">
         <v>59</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -1142,7 +1104,6 @@
       <c r="F24" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="14"/>
       <c r="H24" s="3" t="s">
         <v>67</v>
       </c>
@@ -1158,11 +1119,10 @@
       <c r="L24" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="O24" s="14"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -1175,7 +1135,6 @@
         <v>75</v>
       </c>
       <c r="F25" s="3"/>
-      <c r="G25" s="14"/>
       <c r="H25" s="3"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -1185,16 +1144,14 @@
       <c r="L25" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="O25" s="14"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="14"/>
       <c r="H26" s="3" t="s">
         <v>64</v>
       </c>
@@ -1210,10 +1167,9 @@
       <c r="L26" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="O26" s="14"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
       <c r="D27" t="s">
         <v>17</v>
       </c>
@@ -1227,18 +1183,17 @@
         <v>50</v>
       </c>
       <c r="I27" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="O27" s="14"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>